<commit_message>
update results and figures for revisions with updated Stan version
</commit_message>
<xml_diff>
--- a/results/table_parameters_bare.xlsx
+++ b/results/table_parameters_bare.xlsx
@@ -35,106 +35,106 @@
     <t xml:space="preserve">$\gamma_0$</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.118</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.184</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.413</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.119</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.178</t>
+    <t xml:space="preserve">-0.114</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.190</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.410</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.116</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.187</t>
   </si>
   <si>
     <t xml:space="preserve">$\gamma_1$</t>
   </si>
   <si>
+    <t xml:space="preserve"> 1.027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.131</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.820</t>
+  </si>
+  <si>
     <t xml:space="preserve"> 1.028</t>
   </si>
   <si>
-    <t xml:space="preserve">0.129</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.828</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1.029</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.224</t>
+    <t xml:space="preserve">1.232</t>
   </si>
   <si>
     <t xml:space="preserve">$\gamma_2$</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.060</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.057</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.150</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.059</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.029</t>
+    <t xml:space="preserve">-0.058</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.058</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.148</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.033</t>
   </si>
   <si>
     <t xml:space="preserve">$\gamma_3$</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.077</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.103</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.086</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.236</t>
+    <t xml:space="preserve"> 0.073</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.106</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.096</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.074</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.238</t>
   </si>
   <si>
     <t xml:space="preserve">$\gamma_4$</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.159</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.149</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.354</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.180</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.132</t>
+    <t xml:space="preserve">-0.154</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.157</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.355</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.177</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.159</t>
   </si>
   <si>
     <t xml:space="preserve">$\sigma$</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.092</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.060</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.015</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.083</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.199</t>
+    <t xml:space="preserve"> 0.094</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.064</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.014</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.085</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.206</t>
   </si>
 </sst>
 </file>
@@ -540,27 +540,27 @@
         <v>21</v>
       </c>
       <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
         <v>22</v>
-      </c>
-      <c r="F4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>25</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>26</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>27</v>
-      </c>
-      <c r="E5" t="s">
-        <v>25</v>
       </c>
       <c r="F5" t="s">
         <v>28</v>

</xml_diff>